<commit_message>
Indicadores: CCL; LC; LG; LS;
</commit_message>
<xml_diff>
--- a/Documentos/Calculos/Exemplo calculos.xlsx
+++ b/Documentos/Calculos/Exemplo calculos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'BALANÇO PATRIMONIAL'!$A$2:$D$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DRE!$A$3:$D$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1582,7 +1582,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -1681,7 +1681,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1721,6 +1721,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2057,7 +2063,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2146,6 +2152,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2206,8 +2214,12 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="8" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -2220,6 +2232,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2227,7 +2242,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2265,9 +2280,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2302,7 +2317,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2337,7 +2352,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2532,7 +2547,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>336</v>
       </c>
       <c r="B2" s="26" t="s">
@@ -2540,7 +2555,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="27" t="s">
         <v>413</v>
       </c>
@@ -2593,8 +2608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D183"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2603,12 +2618,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3521,12 +3536,12 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="35" t="s">
+      <c r="A75" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="37"/>
+      <c r="B75" s="38"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="39"/>
     </row>
     <row r="76" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="23" t="s">
@@ -4831,10 +4846,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="21">
@@ -4845,8 +4860,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="42"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="6" t="s">
         <v>411</v>
       </c>
@@ -4855,8 +4870,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="43"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="22">
         <v>42004</v>
       </c>
@@ -5330,7 +5345,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5352,95 +5369,95 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="46" t="s">
         <v>344</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="52" t="s">
         <v>345</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="53">
         <f>(SUM('BALANÇO PATRIMONIAL'!C78,'BALANÇO PATRIMONIAL'!C119) /'BALANÇO PATRIMONIAL'!C157)  * 100</f>
         <v>90.872160385341402</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="50"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="52" t="s">
         <v>346</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="53">
         <f>('BALANÇO PATRIMONIAL'!C78 /SUM('BALANÇO PATRIMONIAL'!C78,'BALANÇO PATRIMONIAL'!C119))  * 100</f>
         <v>37.264824780628082</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="53"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="52" t="s">
         <v>347</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="53">
         <f>(SUM('BALANÇO PATRIMONIAL'!C53,'BALANÇO PATRIMONIAL'!C59,'BALANÇO PATRIMONIAL'!C63)/'BALANÇO PATRIMONIAL'!C157)  * 100</f>
         <v>92.68009720323721</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="53"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="48" t="s">
         <v>348</v>
       </c>
-      <c r="B7" s="47"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="52" t="s">
         <v>349</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="53">
         <f>SUM(INDICADORES!C4,'BALANÇO PATRIMONIAL'!C29)/ SUM('BALANÇO PATRIMONIAL'!C78,'BALANÇO PATRIMONIAL'!C119)</f>
         <v>0.41306936357252638</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="53"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="52" t="s">
         <v>350</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="53">
         <f>'BALANÇO PATRIMONIAL'!C4/'BALANÇO PATRIMONIAL'!C78</f>
         <v>1.7911859081146746</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="53"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="52" t="s">
         <v>351</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="53">
         <f>SUM('BALANÇO PATRIMONIAL'!C5,'BALANÇO PATRIMONIAL'!C6,'BALANÇO PATRIMONIAL'!C12)/'BALANÇO PATRIMONIAL'!C78</f>
         <v>1.3072502063139766</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="53"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="52" t="s">
         <v>352</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="53">
         <f>'BALANÇO PATRIMONIAL'!C4-'BALANÇO PATRIMONIAL'!C78</f>
         <v>1234826</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="53"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="48" t="s">
         <v>353</v>
       </c>
-      <c r="B12" s="47"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="14"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5484,10 +5501,10 @@
       <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="50" t="s">
         <v>358</v>
       </c>
-      <c r="B17" s="49"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5509,7 +5526,7 @@
         <v>86.661230611465868</v>
       </c>
       <c r="C19" s="16"/>
-      <c r="H19" s="51"/>
+      <c r="H19" s="31"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">

</xml_diff>